<commit_message>
Write and read files in encoding determined by CODEPAGE
Close #114, close #115
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_SOXATI4_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_SOXATI4_by_metamake.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">SUBJECT-AREA_da</t>
   </si>
   <si>
-    <t xml:space="preserve">Socialområdet</t>
+    <t xml:space="preserve">SocialomrÃ¥det</t>
   </si>
   <si>
     <t xml:space="preserve">SUBJECT-AREA_kl</t>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">DESCRIPTION_da</t>
   </si>
   <si>
-    <t xml:space="preserve">Arbejdsmarkedsstatus fordelt på uddannelsesniveau &lt;em&gt;[SODATI4]&lt;/em&gt;</t>
+    <t xml:space="preserve">Arbejdsmarkedsstatus fordelt pÃ¥ uddannelsesniveau &lt;em&gt;[SODATI4]&lt;/em&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPTION_kl</t>
@@ -146,7 +146,7 @@
     <t xml:space="preserve">TITLE_da</t>
   </si>
   <si>
-    <t xml:space="preserve">Befolkning efter arbejdsmarkedsstatus, uddannelsesniveau, opgørelsesmetode og tid</t>
+    <t xml:space="preserve">Befolkning efter arbejdsmarkedsstatus, uddannelsesniveau, opgÃ¸relsesmetode og tid</t>
   </si>
   <si>
     <t xml:space="preserve">TITLE_kl</t>
@@ -215,7 +215,7 @@
     <t xml:space="preserve">SOURCE_da</t>
   </si>
   <si>
-    <t xml:space="preserve">Grønlands Statistik</t>
+    <t xml:space="preserve">GrÃ¸nlands Statistik</t>
   </si>
   <si>
     <t xml:space="preserve">SOURCE_kl</t>
@@ -287,7 +287,7 @@
     <t xml:space="preserve">calculation method</t>
   </si>
   <si>
-    <t xml:space="preserve">opgørelsesmetode</t>
+    <t xml:space="preserve">opgÃ¸relsesmetode</t>
   </si>
   <si>
     <t xml:space="preserve">nalunaarsuinermi periuseq</t>
@@ -344,7 +344,7 @@
     <t xml:space="preserve">00 Employed without further details</t>
   </si>
   <si>
-    <t xml:space="preserve">00 Beskæftigede uden nærmere angivelse</t>
+    <t xml:space="preserve">00 BeskÃ¦ftigede uden nÃ¦rmere angivelse</t>
   </si>
   <si>
     <t xml:space="preserve">00 Suliffillit annertunerusumik nalunaarsuuteqanngitsut</t>
@@ -356,7 +356,7 @@
     <t xml:space="preserve">01-02 Employed students</t>
   </si>
   <si>
-    <t xml:space="preserve">01-02 Beskæftigede studerende</t>
+    <t xml:space="preserve">01-02 BeskÃ¦ftigede studerende</t>
   </si>
   <si>
     <t xml:space="preserve">01-02 Ilinniartut suliffillit</t>
@@ -368,7 +368,7 @@
     <t xml:space="preserve">03-04 Employed pensioners</t>
   </si>
   <si>
-    <t xml:space="preserve">03-04 Beskæftigede pensionister</t>
+    <t xml:space="preserve">03-04 BeskÃ¦ftigede pensionister</t>
   </si>
   <si>
     <t xml:space="preserve">03-04 Soraarnerussutisiallit suliffillit</t>
@@ -380,7 +380,7 @@
     <t xml:space="preserve">05-12 Employed with income replacement benefits</t>
   </si>
   <si>
-    <t xml:space="preserve">05-12 Beskæftigede med midlertidigt indkomsterstattende ydelser</t>
+    <t xml:space="preserve">05-12 BeskÃ¦ftigede med midlertidigt indkomsterstattende ydelser</t>
   </si>
   <si>
     <t xml:space="preserve">05-12 Utaqqiisaagallarumik isertitanut taarsiissutaasunik ikiorsiissutinik pisartagallit, ernereernermi pisartagallit ilanngullugit, suliffillit</t>
@@ -452,7 +452,7 @@
     <t xml:space="preserve">70 Children and young people up to and including 15 years of age</t>
   </si>
   <si>
-    <t xml:space="preserve">70 Børn og unge til og med 15 år</t>
+    <t xml:space="preserve">70 BÃ¸rn og unge til og med 15 Ã¥r</t>
   </si>
   <si>
     <t xml:space="preserve">70 Meeqqat 15-inik ataallugilluunniit ukiullit</t>
@@ -464,7 +464,7 @@
     <t xml:space="preserve">90 Others outside the workforce</t>
   </si>
   <si>
-    <t xml:space="preserve">90 Øvrige uden for arbejdsstyrken</t>
+    <t xml:space="preserve">90 Ã˜vrige uden for arbejdsstyrken</t>
   </si>
   <si>
     <t xml:space="preserve">90 Sulisinnaasunut ilaanngitsut allat</t>
@@ -479,7 +479,7 @@
     <t xml:space="preserve">Children and young people up to and including 15 years of age</t>
   </si>
   <si>
-    <t xml:space="preserve">Børn og unge til og med 15 år</t>
+    <t xml:space="preserve">BÃ¸rn og unge til og med 15 Ã¥r</t>
   </si>
   <si>
     <t xml:space="preserve">Meeqqat 15-inik ataallugilluunniit ukiullit</t>
@@ -524,7 +524,7 @@
     <t xml:space="preserve">Post-secondary education</t>
   </si>
   <si>
-    <t xml:space="preserve">Videregående uddanelse</t>
+    <t xml:space="preserve">VideregÃ¥ende uddanelse</t>
   </si>
   <si>
     <t xml:space="preserve">Ingerlariaqqiffiusumik ilinniarfiit</t>
@@ -533,7 +533,7 @@
     <t xml:space="preserve">Annual average, permanent residents</t>
   </si>
   <si>
-    <t xml:space="preserve">Årsgennemsnit, fastboende</t>
+    <t xml:space="preserve">Ã…rsgennemsnit, fastboende</t>
   </si>
   <si>
     <t xml:space="preserve">Najugaqavissut ukiumut agguaqatigiissillugu</t>
@@ -2990,7 +2990,7 @@
     <col min="2" max="2" width="4.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="9.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="64.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="64.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="66.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="144.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="9.71" hidden="0" customWidth="1"/>
   </cols>

</xml_diff>